<commit_message>
Fix corruption in table outputs
</commit_message>
<xml_diff>
--- a/code_examples/excel_from_python/formula_with_tables.xlsx
+++ b/code_examples/excel_from_python/formula_with_tables.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>HSMA T-Shirts</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>HSMA Cat Bowls</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
   <si>
     <t>Item</t>
@@ -79,14 +82,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Stock" displayName="Stock" ref="A1:C4" totalsRowShown="0">
-  <autoFilter ref="A1:C4"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Stock" displayName="Stock" ref="A1:D4" totalsRowShown="0">
+  <autoFilter ref="A1:D4"/>
+  <tableColumns count="4">
     <tableColumn id="1" name="Item"/>
     <tableColumn id="2" name="Units"/>
     <tableColumn id="3" name="Unit Cost"/>
+    <tableColumn id="4" name="Total"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -383,13 +387,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -403,7 +410,7 @@
         <v>11.99</v>
       </c>
       <c r="D2">
-        <f>Stock[@[Units]]*Stock[@[Unit Cost]]</f>
+        <f>B2*C2</f>
         <v>0</v>
       </c>
     </row>
@@ -418,7 +425,7 @@
         <v>0.3</v>
       </c>
       <c r="D3">
-        <f>Stock[@[Units]]*Stock[@[Unit Cost]]</f>
+        <f>B3*C3</f>
         <v>0</v>
       </c>
     </row>
@@ -433,7 +440,7 @@
         <v>15</v>
       </c>
       <c r="D4">
-        <f>Stock[@[Units]]*Stock[@[Unit Cost]]</f>
+        <f>B4*C4</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>